<commit_message>
add TSPPC/TSPCC in the wild experiments
</commit_message>
<xml_diff>
--- a/plot/in_the_wild/comparison_wild.xlsx
+++ b/plot/in_the_wild/comparison_wild.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/in_the_wild/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6641798-D90E-7F4E-A484-B6482777269E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0E6CC4-0BB9-D448-8551-61228C36FB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="timeoverhead_backup" sheetId="3" state="hidden" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="67">
   <si>
     <t>MNIST</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>Memory Usage (KB) - Image</t>
+  </si>
+  <si>
+    <t>TSPPC</t>
+  </si>
+  <si>
+    <t>TSPCC</t>
   </si>
 </sst>
 </file>
@@ -276,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +331,24 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -338,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -383,19 +407,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,12 +750,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="11" t="s">
         <v>22</v>
       </c>
@@ -894,14 +922,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1067,14 +1095,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1120,14 +1148,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1196,12 +1224,12 @@
       <c r="A31" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -1218,14 +1246,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
@@ -1309,7 +1337,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,16 +1348,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1345,6 +1376,13 @@
       <c r="E2" s="11">
         <v>5</v>
       </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1358,6 +1396,15 @@
         <f>C14*E2+C23*E2</f>
         <v>75.773203906250004</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.7005184437500001</v>
+      </c>
+      <c r="I3" s="9">
+        <v>12.88513553125</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1372,21 +1419,21 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B5" s="9">
-        <v>3.4541465312499899</v>
+        <v>3.2025922187499898</v>
       </c>
       <c r="C5" s="9">
-        <v>30.198178593750001</v>
+        <v>27.625677656249898</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
@@ -1421,10 +1468,10 @@
       <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="37">
         <v>0.85</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="37">
         <v>6.05</v>
       </c>
     </row>
@@ -1432,10 +1479,10 @@
       <c r="A11" s="4">
         <v>3</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="37">
         <v>1.6E-2</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="37">
         <v>0.1</v>
       </c>
     </row>
@@ -1443,10 +1490,10 @@
       <c r="A12" s="4">
         <v>4</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="38">
         <v>0.05</v>
       </c>
     </row>
@@ -1475,11 +1522,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -1578,11 +1625,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
@@ -1614,11 +1661,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -1720,11 +1767,11 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
@@ -1823,14 +1870,14 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -1853,17 +1900,18 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="A48:F48"/>
     <mergeCell ref="A1:C1"/>
@@ -1874,6 +1922,7 @@
     <mergeCell ref="A39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1881,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5DAE33-E713-9D41-B622-A5D1F2960391}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1893,16 +1942,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1918,6 +1970,13 @@
       <c r="E2" s="11">
         <v>4</v>
       </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1931,6 +1990,15 @@
         <f>C16*E2+C27*E2</f>
         <v>114.6282655</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0.86387775</v>
+      </c>
+      <c r="I3" s="40">
+        <v>37.243529499999902</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1945,21 +2013,21 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B5" s="9">
-        <v>0.90168174999999995</v>
+        <v>0.86387775</v>
       </c>
       <c r="C5" s="9">
-        <v>38.930881499999998</v>
+        <v>37.243529499999902</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
@@ -2070,11 +2138,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -2199,11 +2267,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -2235,11 +2303,11 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -2363,11 +2431,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
@@ -2492,14 +2560,14 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -2522,17 +2590,18 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="A56:F56"/>
     <mergeCell ref="A58:F58"/>
     <mergeCell ref="A1:C1"/>
@@ -2550,7 +2619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4443E44-1A9C-D84C-8450-192ADD060072}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+    <sheetView zoomScale="136" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2565,19 +2634,19 @@
       <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="2">
@@ -2599,19 +2668,19 @@
       <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="12">
@@ -2639,7 +2708,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2657,13 +2726,13 @@
       <c r="A1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -2809,12 +2878,12 @@
       <c r="A8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2960,12 +3029,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="11" t="s">
         <v>22</v>
       </c>
@@ -3132,14 +3201,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3307,14 +3376,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -3512,14 +3581,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -3565,14 +3634,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -3775,14 +3844,14 @@
       <c r="A47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -3987,12 +4056,12 @@
       <c r="F57" s="14"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -4009,14 +4078,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>

</xml_diff>

<commit_message>
IPSN update remaining evaluation
</commit_message>
<xml_diff>
--- a/plot/in_the_wild/comparison_wild.xlsx
+++ b/plot/in_the_wild/comparison_wild.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/in_the_wild/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E211BF4D-87B9-6649-927D-4905D68AD55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B1E3AA-1F05-7344-8592-64126BF1F193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="4" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
+    <workbookView xWindow="-1400" yWindow="-18220" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="timeoverhead_backup" sheetId="3" state="hidden" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="overhead_image" sheetId="13" r:id="rId3"/>
     <sheet name="memory" sheetId="15" r:id="rId4"/>
     <sheet name="accuracy" sheetId="14" r:id="rId5"/>
-    <sheet name="timeoverhead-task=5" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="overhead_image_pico" sheetId="18" r:id="rId6"/>
+    <sheet name="timeoverhead-task=5" sheetId="5" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,9 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="69">
   <si>
     <t>MNIST</t>
   </si>
@@ -239,6 +243,12 @@
   </si>
   <si>
     <t>TSPCC</t>
+  </si>
+  <si>
+    <t>Pico</t>
+  </si>
+  <si>
+    <t>Portenta</t>
   </si>
 </sst>
 </file>
@@ -1928,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5DAE33-E713-9D41-B622-A5D1F2960391}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1947,9 +1957,10 @@
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
-      <c r="D1" s="27"/>
+      <c r="D1" s="27" t="s">
+        <v>68</v>
+      </c>
       <c r="E1" s="27"/>
-      <c r="F1" s="19"/>
       <c r="G1" s="40" t="s">
         <v>65</v>
       </c>
@@ -1983,21 +1994,26 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <f>B16*E2+B27*E2</f>
-        <v>2.67614975</v>
+        <f>B9/16.57</f>
+        <v>0.16150571816535908</v>
       </c>
       <c r="C3" s="9">
-        <f>C16*E2+C27*E2</f>
-        <v>114.6282655</v>
+        <f>B3*99.6</f>
+        <v>16.085969529269764</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H3" s="37">
-        <v>0.86387775</v>
+        <f>H4/16.57</f>
+        <v>5.2135048280024139E-2</v>
       </c>
       <c r="I3" s="37">
-        <v>37.243529499999902</v>
+        <f>H3*99.6</f>
+        <v>5.192650808690404</v>
+      </c>
+      <c r="J3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2005,10 +2021,24 @@
         <v>11</v>
       </c>
       <c r="B4" s="9">
-        <v>1.7154467499999999</v>
+        <f t="shared" ref="B4:C5" si="0">B10/16.57</f>
+        <v>0.10352726312613156</v>
       </c>
       <c r="C4" s="9">
-        <v>73.9504515</v>
+        <f t="shared" ref="C4:C5" si="1">B4*99.6</f>
+        <v>10.311315407362702</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="37">
+        <v>0.86387775</v>
+      </c>
+      <c r="I4" s="37">
+        <v>37.243529499999902</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2016,600 +2046,664 @@
         <v>61</v>
       </c>
       <c r="B5" s="9">
-        <v>0.86387775</v>
+        <f t="shared" si="0"/>
+        <v>5.2135048280024139E-2</v>
       </c>
       <c r="C5" s="9">
-        <v>37.243529499999902</v>
+        <f t="shared" si="1"/>
+        <v>5.192650808690404</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="27"/>
       <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <f>B22*E8+B33*E8</f>
+        <v>2.67614975</v>
+      </c>
+      <c r="C9" s="9">
+        <f>C22*E8+C33*E8</f>
+        <v>114.6282655</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1.7154467499999999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>73.9504515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.86387775</v>
+      </c>
+      <c r="C11" s="9">
+        <v>37.243529499999902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C14" s="20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.24</v>
-      </c>
-      <c r="C9" s="5">
-        <v>10.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.22</v>
-      </c>
-      <c r="C10" s="5">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3.82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B15" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>0.24</v>
       </c>
       <c r="C15" s="5">
-        <v>0.13</v>
+        <v>10.16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16">
-        <f>SUM(B9:B15)</f>
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="C16" s="16">
-        <f>SUM(C9:C15)</f>
-        <v>26.88</v>
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="C16" s="5">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3.82</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
+      <c r="A18" s="4">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>31</v>
+      <c r="A19" s="4">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.59</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="9">
-        <f>D57/B57*B47</f>
-        <v>1.7574999999999999E-4</v>
-      </c>
-      <c r="C20" s="9">
-        <f>F57/B57*C47</f>
-        <v>9.4535000000000001E-3</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>2</v>
-      </c>
-      <c r="B21" s="9">
-        <f>D57/B57*B48</f>
-        <v>6.9349999999999989E-4</v>
-      </c>
-      <c r="C21" s="9">
-        <f>F57/B57*C48</f>
-        <v>3.7302999999999996E-2</v>
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.13</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>3</v>
-      </c>
-      <c r="B22" s="9">
-        <f>D57/B57*B49</f>
-        <v>2.7549999999999996E-3</v>
-      </c>
-      <c r="C22" s="9">
-        <f>F57/B57*C49</f>
-        <v>0.14818999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>4</v>
-      </c>
-      <c r="B23" s="9">
-        <f>D57/B57*B50</f>
-        <v>1.9494000000000001E-2</v>
-      </c>
-      <c r="C23" s="9">
-        <f>F57/B57*C50</f>
-        <v>1.0485720000000001</v>
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="16">
+        <f>SUM(B15:B21)</f>
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="C22" s="16">
+        <f>SUM(C15:C21)</f>
+        <v>26.88</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>5</v>
-      </c>
-      <c r="B24" s="9">
-        <f>D57/B57*B51</f>
-        <v>4.9399999999999999E-3</v>
-      </c>
-      <c r="C24" s="9">
-        <f>F57/B57*C51</f>
-        <v>0.26572000000000001</v>
-      </c>
+      <c r="A24" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>6</v>
-      </c>
-      <c r="B25" s="9">
-        <f>D57/B57*B52</f>
-        <v>4.9020000000000001E-3</v>
-      </c>
-      <c r="C25" s="9">
-        <f>F57/B57*C52</f>
-        <v>0.26367600000000002</v>
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <f>D63/B63*B53</f>
+        <v>1.7574999999999999E-4</v>
+      </c>
+      <c r="C26" s="9">
+        <f>F63/B63*C53</f>
+        <v>9.4535000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27" s="9">
+        <f>D63/B63*B54</f>
+        <v>6.9349999999999989E-4</v>
+      </c>
+      <c r="C27" s="9">
+        <f>F63/B63*C54</f>
+        <v>3.7302999999999996E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>3</v>
+      </c>
+      <c r="B28" s="9">
+        <f>D63/B63*B55</f>
+        <v>2.7549999999999996E-3</v>
+      </c>
+      <c r="C28" s="9">
+        <f>F63/B63*C55</f>
+        <v>0.14818999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>4</v>
+      </c>
+      <c r="B29" s="9">
+        <f>D63/B63*B56</f>
+        <v>1.9494000000000001E-2</v>
+      </c>
+      <c r="C29" s="9">
+        <f>F63/B63*C56</f>
+        <v>1.0485720000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>5</v>
+      </c>
+      <c r="B30" s="9">
+        <f>D63/B63*B57</f>
+        <v>4.9399999999999999E-3</v>
+      </c>
+      <c r="C30" s="9">
+        <f>F63/B63*C57</f>
+        <v>0.26572000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>6</v>
+      </c>
+      <c r="B31" s="9">
+        <f>D63/B63*B58</f>
+        <v>4.9020000000000001E-3</v>
+      </c>
+      <c r="C31" s="9">
+        <f>F63/B63*C58</f>
+        <v>0.26367600000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>7</v>
       </c>
-      <c r="B26" s="9">
-        <f>D57/B57*B53</f>
+      <c r="B32" s="9">
+        <f>D63/B63*B59</f>
         <v>7.7187499999999999E-5</v>
       </c>
-      <c r="C26" s="9">
-        <f>F57/B57*C53</f>
+      <c r="C32" s="9">
+        <f>F63/B63*C59</f>
         <v>4.1518750000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="9">
-        <f>SUM(B20:B26)</f>
+      <c r="B33" s="9">
+        <f>SUM(B26:B32)</f>
         <v>3.3037437499999996E-2</v>
       </c>
-      <c r="C27" s="9">
-        <f>SUM(C20:C26)</f>
+      <c r="C33" s="9">
+        <f>SUM(C26:C32)</f>
         <v>1.777066375</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="38" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="23" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C36" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="9">
-        <f>D57/B57*B54</f>
+      <c r="B37" s="9">
+        <f>D63/B63*B60</f>
         <v>3.3037437500000003E-2</v>
       </c>
-      <c r="C31" s="9">
-        <f>F57/B57*C54</f>
+      <c r="C37" s="9">
+        <f>F63/B63*C60</f>
         <v>1.7770663750000002</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B40" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C40" s="22" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5">
-        <v>296</v>
-      </c>
-      <c r="C35" s="5">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
-        <v>2</v>
-      </c>
-      <c r="B36" s="5">
-        <v>1168</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
-        <v>3</v>
-      </c>
-      <c r="B37" s="5">
-        <v>4640</v>
-      </c>
-      <c r="C37" s="5">
-        <v>4640</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>4</v>
-      </c>
-      <c r="B38" s="5">
-        <v>32832</v>
-      </c>
-      <c r="C38" s="5">
-        <v>32832</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
-        <v>5</v>
-      </c>
-      <c r="B39" s="5">
-        <v>8320</v>
-      </c>
-      <c r="C39" s="5">
-        <v>8320</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
-        <v>6</v>
-      </c>
-      <c r="B40" s="5">
-        <v>8256</v>
-      </c>
-      <c r="C40" s="5">
-        <v>8256</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B41" s="5">
-        <v>130</v>
+        <v>296</v>
       </c>
       <c r="C41" s="5">
-        <v>130</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="21">
-        <f>SUM(B35:B41)</f>
-        <v>55642</v>
-      </c>
-      <c r="C42" s="21">
-        <f>SUM(C35:C41)</f>
-        <v>55642</v>
+      <c r="A42" s="4">
+        <v>2</v>
+      </c>
+      <c r="B42" s="5">
+        <v>1168</v>
+      </c>
+      <c r="C42" s="5">
+        <v>1168</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="21">
-        <f>B42*2/1000</f>
-        <v>111.28400000000001</v>
-      </c>
-      <c r="C43" s="21">
-        <f>C42*2/1000</f>
-        <v>111.28400000000001</v>
+      <c r="A43" s="4">
+        <v>3</v>
+      </c>
+      <c r="B43" s="5">
+        <v>4640</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>4</v>
+      </c>
+      <c r="B44" s="5">
+        <v>32832</v>
+      </c>
+      <c r="C44" s="5">
+        <v>32832</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="A45" s="4">
+        <v>5</v>
+      </c>
+      <c r="B45" s="5">
+        <v>8320</v>
+      </c>
+      <c r="C45" s="5">
+        <v>8320</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>31</v>
+      <c r="A46" s="4">
+        <v>6</v>
+      </c>
+      <c r="B46" s="5">
+        <v>8256</v>
+      </c>
+      <c r="C46" s="5">
+        <v>8256</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
+        <v>7</v>
+      </c>
+      <c r="B47" s="5">
+        <v>130</v>
+      </c>
+      <c r="C47" s="5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="21">
+        <f>SUM(B41:B47)</f>
+        <v>55642</v>
+      </c>
+      <c r="C48" s="21">
+        <f>SUM(C41:C47)</f>
+        <v>55642</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="21">
+        <f>B48*2/1000</f>
+        <v>111.28400000000001</v>
+      </c>
+      <c r="C49" s="21">
+        <f>C48*2/1000</f>
+        <v>111.28400000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
         <v>1</v>
       </c>
-      <c r="B47" s="9">
-        <f t="shared" ref="B47:C52" si="0">B35*2/1000</f>
+      <c r="B53" s="9">
+        <f t="shared" ref="B53:C58" si="2">B41*2/1000</f>
         <v>0.59199999999999997</v>
       </c>
-      <c r="C47" s="9">
-        <f t="shared" si="0"/>
+      <c r="C53" s="9">
+        <f t="shared" si="2"/>
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
         <v>2</v>
       </c>
-      <c r="B48" s="9">
-        <f t="shared" si="0"/>
+      <c r="B54" s="9">
+        <f t="shared" si="2"/>
         <v>2.3359999999999999</v>
       </c>
-      <c r="C48" s="9">
-        <f t="shared" si="0"/>
+      <c r="C54" s="9">
+        <f t="shared" si="2"/>
         <v>2.3359999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
         <v>3</v>
       </c>
-      <c r="B49" s="9">
-        <f t="shared" si="0"/>
+      <c r="B55" s="9">
+        <f t="shared" si="2"/>
         <v>9.2799999999999994</v>
       </c>
-      <c r="C49" s="9">
-        <f t="shared" si="0"/>
+      <c r="C55" s="9">
+        <f t="shared" si="2"/>
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
         <v>4</v>
       </c>
-      <c r="B50" s="9">
-        <f t="shared" si="0"/>
+      <c r="B56" s="9">
+        <f t="shared" si="2"/>
         <v>65.664000000000001</v>
       </c>
-      <c r="C50" s="9">
-        <f t="shared" si="0"/>
+      <c r="C56" s="9">
+        <f t="shared" si="2"/>
         <v>65.664000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
         <v>5</v>
       </c>
-      <c r="B51" s="9">
-        <f t="shared" si="0"/>
+      <c r="B57" s="9">
+        <f t="shared" si="2"/>
         <v>16.64</v>
       </c>
-      <c r="C51" s="9">
-        <f t="shared" si="0"/>
+      <c r="C57" s="9">
+        <f t="shared" si="2"/>
         <v>16.64</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
         <v>6</v>
       </c>
-      <c r="B52" s="9">
-        <f t="shared" si="0"/>
+      <c r="B58" s="9">
+        <f t="shared" si="2"/>
         <v>16.512</v>
       </c>
-      <c r="C52" s="9">
-        <f t="shared" si="0"/>
+      <c r="C58" s="9">
+        <f t="shared" si="2"/>
         <v>16.512</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
         <v>7</v>
       </c>
-      <c r="B53" s="9">
-        <f>B41*2/1000</f>
+      <c r="B59" s="9">
+        <f>B47*2/1000</f>
         <v>0.26</v>
       </c>
-      <c r="C53" s="9">
-        <f t="shared" ref="C53" si="1">C41*2/1000</f>
+      <c r="C59" s="9">
+        <f t="shared" ref="C59" si="3">C47*2/1000</f>
         <v>0.26</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="9">
-        <f>SUM(B47:B53)</f>
+      <c r="B60" s="9">
+        <f>SUM(B53:B59)</f>
         <v>111.28400000000001</v>
       </c>
-      <c r="C54" s="9">
-        <f>SUM(C47:C53)</f>
+      <c r="C60" s="9">
+        <f>SUM(C53:C59)</f>
         <v>111.28400000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="38" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B63" s="9">
         <v>64</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D63" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F63" s="2">
         <v>1.022</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A64:F64"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2707,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CB3D5B-1142-B443-8081-E5AC18776E24}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+    <sheetView zoomScale="132" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -3016,6 +3110,695 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185A345E-5CFC-8048-892D-99F6BA2AA080}">
+  <dimension ref="A1:J58"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="11">
+        <v>4</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <f>B16*E2+B27*E2</f>
+        <v>2.67614975</v>
+      </c>
+      <c r="C3" s="9">
+        <f>C16*E2+C27*E2</f>
+        <v>114.6282655</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="37">
+        <v>0.86387775</v>
+      </c>
+      <c r="I3" s="37">
+        <v>37.243529499999902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1.7154467499999999</v>
+      </c>
+      <c r="C4" s="9">
+        <v>73.9504515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.86387775</v>
+      </c>
+      <c r="C5" s="9">
+        <v>37.243529499999902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="C9" s="5">
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="C10" s="5">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16">
+        <f>SUM(B9:B15)</f>
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="C16" s="16">
+        <f>SUM(C9:C15)</f>
+        <v>26.88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <f>D57/B57*B47</f>
+        <v>1.7574999999999999E-4</v>
+      </c>
+      <c r="C20" s="9">
+        <f>F57/B57*C47</f>
+        <v>9.4535000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="9">
+        <f>D57/B57*B48</f>
+        <v>6.9349999999999989E-4</v>
+      </c>
+      <c r="C21" s="9">
+        <f>F57/B57*C48</f>
+        <v>3.7302999999999996E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9">
+        <f>D57/B57*B49</f>
+        <v>2.7549999999999996E-3</v>
+      </c>
+      <c r="C22" s="9">
+        <f>F57/B57*C49</f>
+        <v>0.14818999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>4</v>
+      </c>
+      <c r="B23" s="9">
+        <f>D57/B57*B50</f>
+        <v>1.9494000000000001E-2</v>
+      </c>
+      <c r="C23" s="9">
+        <f>F57/B57*C50</f>
+        <v>1.0485720000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>5</v>
+      </c>
+      <c r="B24" s="9">
+        <f>D57/B57*B51</f>
+        <v>4.9399999999999999E-3</v>
+      </c>
+      <c r="C24" s="9">
+        <f>F57/B57*C51</f>
+        <v>0.26572000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>6</v>
+      </c>
+      <c r="B25" s="9">
+        <f>D57/B57*B52</f>
+        <v>4.9020000000000001E-3</v>
+      </c>
+      <c r="C25" s="9">
+        <f>F57/B57*C52</f>
+        <v>0.26367600000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>7</v>
+      </c>
+      <c r="B26" s="9">
+        <f>D57/B57*B53</f>
+        <v>7.7187499999999999E-5</v>
+      </c>
+      <c r="C26" s="9">
+        <f>F57/B57*C53</f>
+        <v>4.1518750000000002E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="9">
+        <f>SUM(B20:B26)</f>
+        <v>3.3037437499999996E-2</v>
+      </c>
+      <c r="C27" s="9">
+        <f>SUM(C20:C26)</f>
+        <v>1.777066375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="9">
+        <f>D57/B57*B54</f>
+        <v>3.3037437500000003E-2</v>
+      </c>
+      <c r="C31" s="9">
+        <f>F57/B57*C54</f>
+        <v>1.7770663750000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
+        <v>296</v>
+      </c>
+      <c r="C35" s="5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>2</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1168</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5">
+        <v>4640</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5">
+        <v>32832</v>
+      </c>
+      <c r="C38" s="5">
+        <v>32832</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>5</v>
+      </c>
+      <c r="B39" s="5">
+        <v>8320</v>
+      </c>
+      <c r="C39" s="5">
+        <v>8320</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>6</v>
+      </c>
+      <c r="B40" s="5">
+        <v>8256</v>
+      </c>
+      <c r="C40" s="5">
+        <v>8256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>7</v>
+      </c>
+      <c r="B41" s="5">
+        <v>130</v>
+      </c>
+      <c r="C41" s="5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="21">
+        <f>SUM(B35:B41)</f>
+        <v>55642</v>
+      </c>
+      <c r="C42" s="21">
+        <f>SUM(C35:C41)</f>
+        <v>55642</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="21">
+        <f>B42*2/1000</f>
+        <v>111.28400000000001</v>
+      </c>
+      <c r="C43" s="21">
+        <f>C42*2/1000</f>
+        <v>111.28400000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>1</v>
+      </c>
+      <c r="B47" s="9">
+        <f t="shared" ref="B47:C53" si="0">B35*2/1000</f>
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="C47" s="9">
+        <f t="shared" si="0"/>
+        <v>0.59199999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>2</v>
+      </c>
+      <c r="B48" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="C48" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3359999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>3</v>
+      </c>
+      <c r="B49" s="9">
+        <f t="shared" si="0"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="C49" s="9">
+        <f t="shared" si="0"/>
+        <v>9.2799999999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>4</v>
+      </c>
+      <c r="B50" s="9">
+        <f t="shared" si="0"/>
+        <v>65.664000000000001</v>
+      </c>
+      <c r="C50" s="9">
+        <f t="shared" si="0"/>
+        <v>65.664000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>5</v>
+      </c>
+      <c r="B51" s="9">
+        <f t="shared" si="0"/>
+        <v>16.64</v>
+      </c>
+      <c r="C51" s="9">
+        <f t="shared" si="0"/>
+        <v>16.64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>6</v>
+      </c>
+      <c r="B52" s="9">
+        <f t="shared" si="0"/>
+        <v>16.512</v>
+      </c>
+      <c r="C52" s="9">
+        <f t="shared" si="0"/>
+        <v>16.512</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>7</v>
+      </c>
+      <c r="B53" s="9">
+        <f>B41*2/1000</f>
+        <v>0.26</v>
+      </c>
+      <c r="C53" s="9">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="9">
+        <f>SUM(B47:B53)</f>
+        <v>111.28400000000001</v>
+      </c>
+      <c r="C54" s="9">
+        <f>SUM(C47:C53)</f>
+        <v>111.28400000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="9">
+        <v>64</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1.022</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A33:C33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BB6D28-0DA4-6B47-9767-B86832CEED60}">
   <dimension ref="A1:F66"/>
   <sheetViews>

</xml_diff>